<commit_message>
Removed CN command from all data feeds.
</commit_message>
<xml_diff>
--- a/Settings/Base/005_BaseRegionClassification.xlsx
+++ b/Settings/Base/005_BaseRegionClassification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hwieland\Github workspace\PIOLab\ConcordanceLibrary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hwieland\Github workspace\PIOLab\Settings\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Code</t>
   </si>
@@ -45,6 +45,21 @@
   </si>
   <si>
     <t>RoW</t>
+  </si>
+  <si>
+    <t>Abbrev</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>AU</t>
   </si>
 </sst>
 </file>
@@ -381,10 +396,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -392,82 +407,100 @@
     <col min="1" max="1" width="5.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">
@@ -571,5 +604,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>